<commit_message>
Thanks For 鹿and犀 to add three png base map
</commit_message>
<xml_diff>
--- a/DataFileSamples/TAS REE Trace Pearce Harker CIPW/Data.xlsx
+++ b/DataFileSamples/TAS REE Trace Pearce Harker CIPW/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cycleuser/Documents/GitHub/GeoPyTool/DataFileSamples/TAS REE Trace Pearce Harker CIPW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{580AC540-782F-CF4A-93CA-A77AD75911BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D27927B2-903E-A947-95E8-DC91D209C4FA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="460" windowWidth="21600" windowHeight="18960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
@@ -989,13 +989,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="7" max="7" width="30.5" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59">

</xml_diff>